<commit_message>
update raw data - we included the VT from the July prague trip. VT 13 and 14.
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-I-rove_time.xlsx
+++ b/data/raw/VCAS-I-rove_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B15437C-21D8-9E45-A8B6-02E13D025CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75A45FF-A20F-484F-BBAD-697EA6F95F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <sheet name="1-010" sheetId="15" r:id="rId6"/>
     <sheet name="1-012" sheetId="17" r:id="rId7"/>
     <sheet name="1-013" sheetId="16" r:id="rId8"/>
-    <sheet name="template" sheetId="11" r:id="rId9"/>
+    <sheet name="1-014" sheetId="19" r:id="rId9"/>
+    <sheet name="1-015" sheetId="18" r:id="rId10"/>
+    <sheet name="template" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="84">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -94,9 +96,6 @@
     <t>https://www.dropbox.com/scl/fo/q1tba9iyynwoeceh8qfv3/APyARUVqai82OSEcUvw0p1g?rlkey=noxj9yewkgsqrboh2kexjftyd&amp;st=yae78lfa&amp;dl=0</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/scl/fo/lgbfgrdztyqibgbmd37jf/AJgChytFd4m-vdmPyFqWyTs?rlkey=nvxzk4jz0hrbebfmb9t4i0seq&amp;st=nc76hmfo&amp;dl=0</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -169,16 +168,7 @@
     <t>Targetting that annuluar exit that's hard to reach</t>
   </si>
   <si>
-    <t>https://fieldmedical.sharepoint.com/:f:/r/sites/Clinical/Shared%20Documents/FIM%20Recorded%20Cases/VCAS%20Pt%201-004%20through%201-009/case%202%20-%201-005?csf=1&amp;web=1&amp;e=WrvKUw</t>
-  </si>
-  <si>
     <t>stopped to remap</t>
-  </si>
-  <si>
-    <t>incomplete footage? It's only 30ish min and shows a couple lesions, but there should be 19</t>
-  </si>
-  <si>
-    <t>no more footage? This was too short, there should have been more lesions</t>
   </si>
   <si>
     <t>stops for induction/remapping</t>
@@ -383,6 +373,57 @@
       </rPr>
       <t xml:space="preserve"> stop the timer, this is a PFA specific time sink</t>
     </r>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/5tyj68sp7zxyd2jq5jweo/mapping_1.mp4?rlkey=z7xmuub9432pvl1mj980fkxzl&amp;st=ma5rfzyj&amp;dl=0</t>
+  </si>
+  <si>
+    <t>Do not have vascular access - skin closure time</t>
+  </si>
+  <si>
+    <t>1-014</t>
+  </si>
+  <si>
+    <t>1-015</t>
+  </si>
+  <si>
+    <t>only 2 lesions then remap</t>
+  </si>
+  <si>
+    <t>annular lesions then remap</t>
+  </si>
+  <si>
+    <t>Next lesions on mapping_2 videos. Case was split up between two sets of videos</t>
+  </si>
+  <si>
+    <t>15kv_20x5_uni</t>
+  </si>
+  <si>
+    <t>15kv_3x12_uni</t>
+  </si>
+  <si>
+    <t>therapy</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fo/wqvpzty7er5co1je1q5a8/AGeRgYaALyUJ7ocLsmvpQys?rlkey=jvtr1ahy8gjngyvz6c77k6ue6&amp;st=ai1fvbnr&amp;dl=0</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fo/is570gcktbtom1msir8zt/AONNAhFHaPlLnkOqadXyaqY?rlkey=z19u932s4tm1gc9ahuyoehpmk&amp;st=us60wflb&amp;dl=0</t>
+  </si>
+  <si>
+    <t>Why did we give so many single application lesions in this case?</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fo/xhk78kalk65wgpvj7auyb/AE_ARhwxc15CqbcynuscspI?rlkey=y43fcxabmq98k6b0bd886gy5s&amp;st=2183dxy9&amp;dl=0</t>
+  </si>
+  <si>
+    <t>Ablation 1 and 2 during VT. Got through 4 lesions before stopping to troubleshoot.</t>
+  </si>
+  <si>
+    <t>stop to remap - induced VT and mapped it more basal</t>
+  </si>
+  <si>
+    <t>map and term during VT2</t>
   </si>
 </sst>
 </file>
@@ -449,7 +490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -457,11 +498,7 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -469,7 +506,25 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
     </dxf>
@@ -540,6 +595,9 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
@@ -556,15 +614,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:F33" totalsRowShown="0">
-  <autoFilter ref="A1:F33" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:G33" totalsRowShown="0">
+  <autoFilter ref="A1:G33" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{A7F69E93-3952-2D4F-B01B-B9EB9DC3432C}" name="link_to_data"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}" name="Table24" displayName="Table24" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="0">
+      <calculatedColumnFormula>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{5466BD7A-7146-7E49-B844-B14DB335F671}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -576,7 +650,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{01F56379-480D-E144-8844-79E29F338160}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{80A1EC3F-97BF-2A42-A823-A672AD58C802}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="24">
       <calculatedColumnFormula>Table2[[#This Row],[end_time]]-Table2[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DC0F7FFE-563B-3E40-AAB4-A68B98253F92}" name="notes"/>
@@ -589,9 +663,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAC55445-B449-1B46-ADAD-5D1EE6A1BD3D}" name="Table246" displayName="Table246" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="21">
       <calculatedColumnFormula>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{838825F0-239B-C440-9C0B-3A9D1E9C0D95}" name="notes"/>
@@ -604,9 +678,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7DEA103-B67A-0B49-99E5-BEE70970D4BB}" name="Table247" displayName="Table247" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="18">
       <calculatedColumnFormula>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{CCA0740F-5707-C44E-AA57-B44DAE132805}" name="notes"/>
@@ -619,9 +693,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{772A68B7-3577-954E-96AB-3F9F135762FE}" name="Table248" displayName="Table248" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="15">
       <calculatedColumnFormula>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F22060DE-01C3-9C4C-A473-BCE8D37580D6}" name="notes"/>
@@ -634,9 +708,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D84B3EF0-7875-184B-870A-3642242A31F0}" name="Table2410" displayName="Table2410" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="12">
       <calculatedColumnFormula>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7A57ED91-2446-8F4F-95C2-3088CD96BD62}" name="notes"/>
@@ -649,9 +723,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A3CEC53-F376-1D4D-846C-0F34B09239B4}" name="Table249" displayName="Table249" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="9">
       <calculatedColumnFormula>Table249[[#This Row],[end_time]]-Table249[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7880A518-97D3-0D44-977A-E75D9468AB4A}" name="notes"/>
@@ -661,15 +735,30 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}" name="Table24" displayName="Table24" ref="A1:D31" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A7ADDBBE-0483-F84D-98C5-791E3CFC3CE4}" name="Table24511" displayName="Table24511" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="0">
-      <calculatedColumnFormula>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="6">
+      <calculatedColumnFormula>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5466BD7A-7146-7E49-B844-B14DB335F671}" name="notes"/>
+    <tableColumn id="4" xr3:uid="{6BF25E36-BEFE-334C-B53B-9359DA68008A}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{039AD6AB-0126-1947-A333-DE36DDA0B7E4}" name="Table245" displayName="Table245" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="3">
+      <calculatedColumnFormula>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F8493A5C-0C25-FD45-A552-FE369F4F3DAD}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -994,25 +1083,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535426F-7A8C-E949-810F-FB71A9FDBD02}">
   <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView zoomScale="179" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -1022,27 +1111,27 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -1056,53 +1145,53 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1110,43 +1199,709 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88A8D6D-D290-9244-9467-AD71E2C0964F}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>0.77465277777777775</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.78122685185185181</v>
+      </c>
+      <c r="C2" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>6.5740740740740655E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4">
+        <f>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="6">
+        <f>HOUR(SUM(Table245[time_diff]))*3600 + MINUTE(SUM(Table245[time_diff])) * 60 + SECOND(SUM(Table245[time_diff]))</f>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.69097222222222221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6">
+        <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
+        <v>9600</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5D0936-41CB-4D48-9AD9-6C4AF0186848}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="C2" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4">
+        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="6">
+        <f>HOUR(SUM(Table24[time_diff]))*3600 + MINUTE(SUM(Table24[time_diff])) * 60 + SECOND(SUM(Table24[time_diff]))</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6">
+        <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView zoomScale="201" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
+        <v>52</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1159,14 +1914,17 @@
       <c r="D2" s="6">
         <v>77</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1179,26 +1937,35 @@
       <c r="D3" s="6">
         <v>165</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="E3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C4" s="6">
+        <v>2075</v>
+      </c>
+      <c r="D4" s="6">
+        <v>95</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1212,23 +1979,26 @@
       <c r="D5" s="6">
         <v>75</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1241,12 +2011,15 @@
       <c r="D7" s="6">
         <v>102</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1259,126 +2032,167 @@
       <c r="D8" s="6">
         <v>31</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="6">
+        <v>12840</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2043</v>
+      </c>
+      <c r="D9" s="6">
+        <v>105</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="6">
+        <v>9600</v>
+      </c>
+      <c r="C10" s="6">
+        <v>568</v>
+      </c>
+      <c r="D10" s="6">
+        <v>35</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E37" s="4"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
-    <hyperlink ref="F5" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
+    <hyperlink ref="G9" r:id="rId7" xr:uid="{3DBA40E2-94AD-4845-AA90-D92036F9A7B1}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{53E20B43-9ECF-BE46-AB3C-B2592713D701}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1400,16 +2214,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1424,7 +2238,7 @@
         <v>4.6296296296294281E-5</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1439,7 +2253,7 @@
         <v>4.398148148148151E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1454,7 +2268,7 @@
         <v>2.1504629629629637E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1469,7 +2283,7 @@
         <v>5.7870370370372015E-4</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1484,7 +2298,7 @@
         <v>3.4722222222222099E-4</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1499,7 +2313,7 @@
         <v>5.5439814814814969E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1648,7 +2462,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2[time_diff]))*3600 + MINUTE(SUM(Table2[time_diff])) * 60 + SECOND(SUM(Table2[time_diff]))</f>
@@ -1657,13 +2471,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5">
         <v>0.37847222222222221</v>
@@ -1671,7 +2485,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <v>0.62847222222222221</v>
@@ -1679,14 +2493,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
         <v>21600</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1712,16 +2526,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1736,7 +2550,7 @@
         <v>3.0902777777777751E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1751,7 +2565,7 @@
         <v>4.4212962962962843E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1766,7 +2580,7 @@
         <v>2.6423611111111134E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1781,7 +2595,7 @@
         <v>6.481481481481477E-4</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1796,7 +2610,7 @@
         <v>4.2824074074074292E-4</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2001,7 +2815,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table246[time_diff]))*3600 + MINUTE(SUM(Table246[time_diff])) * 60 + SECOND(SUM(Table246[time_diff]))</f>
@@ -2010,13 +2824,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5">
         <v>0.40277777777777779</v>
@@ -2024,7 +2838,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <v>0.46805555555555556</v>
@@ -2032,14 +2846,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
         <v>5640</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +2869,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2065,58 +2879,76 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>3.8657407407407408E-3</v>
+        <v>0.64217592592592587</v>
       </c>
       <c r="B2" s="5">
-        <v>6.7939814814814816E-3</v>
+        <v>0.65585648148148146</v>
       </c>
       <c r="C2" s="4">
         <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>2.9282407407407408E-3</v>
+        <v>1.3680555555555585E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="5">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.67078703703703701</v>
+      </c>
       <c r="C3" s="4">
         <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <v>1.3425925925926174E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="5">
+        <v>0.68248842592592596</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.68859953703703702</v>
+      </c>
       <c r="C4" s="4">
         <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <v>6.1111111111110672E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="5">
+        <v>3.8310185185185183E-3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>6.7129629629629631E-3</v>
+      </c>
       <c r="C5" s="4">
         <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <v>2.8819444444444448E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2329,22 +3161,22 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table247[time_diff]))*3600 + MINUTE(SUM(Table247[time_diff])) * 60 + SECOND(SUM(Table247[time_diff]))</f>
-        <v>253</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5">
         <v>0</v>
@@ -2352,7 +3184,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <v>0</v>
@@ -2360,14 +3192,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2393,16 +3225,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2417,7 +3249,7 @@
         <v>2.6851851851851863E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2662,7 +3494,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table248[time_diff]))*3600 + MINUTE(SUM(Table248[time_diff])) * 60 + SECOND(SUM(Table248[time_diff]))</f>
@@ -2671,13 +3503,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5">
         <v>0.36527777777777776</v>
@@ -2685,7 +3517,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <v>0.5708333333333333</v>
@@ -2693,14 +3525,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
         <v>17760</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2726,16 +3558,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2750,7 +3582,7 @@
         <v>1.0798611111111113E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2765,7 +3597,7 @@
         <v>7.5578703703703745E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2780,7 +3612,7 @@
         <v>1.4004629629629645E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2795,7 +3627,7 @@
         <v>3.1250000000000722E-4</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3008,7 +3840,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2410[time_diff]))*3600 + MINUTE(SUM(Table2410[time_diff])) * 60 + SECOND(SUM(Table2410[time_diff]))</f>
@@ -3017,13 +3849,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5">
         <v>0.44583333333333336</v>
@@ -3031,7 +3863,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <v>0.54861111111111116</v>
@@ -3039,14 +3871,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
         <v>8880</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3072,16 +3904,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3346,7 +4178,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table249[time_diff]))*3600 + MINUTE(SUM(Table249[time_diff])) * 60 + SECOND(SUM(Table249[time_diff]))</f>
@@ -3355,13 +4187,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5">
         <v>0.61388888888888893</v>
@@ -3369,7 +4201,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <v>0.71527777777777779</v>
@@ -3377,14 +4209,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
         <v>8760</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3396,11 +4228,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5D0936-41CB-4D48-9AD9-6C4AF0186848}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E96B43-315A-A34D-AC7F-DA126C47C92D}">
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3410,52 +4242,73 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>6.9444444444444447E-4</v>
+        <v>0.55614583333333334</v>
       </c>
       <c r="B2" s="5">
-        <v>1.3888888888888889E-3</v>
+        <v>0.56443287037037038</v>
       </c>
       <c r="C2" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
-        <v>6.9444444444444447E-4</v>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>8.2870370370370372E-3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="5">
+        <v>0.57165509259259262</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.57843750000000005</v>
+      </c>
       <c r="C3" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>6.7824074074074314E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="5">
+        <v>0.58763888888888893</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.59467592592592589</v>
+      </c>
       <c r="C4" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>7.0370370370369528E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="5">
+        <v>0.60098379629629628</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.60252314814814811</v>
+      </c>
       <c r="C5" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>1.5393518518518334E-3</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -3463,7 +4316,7 @@
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3471,7 +4324,7 @@
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
       <c r="G7" s="5"/>
@@ -3480,7 +4333,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3488,7 +4341,7 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3496,7 +4349,7 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3504,7 +4357,7 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3512,7 +4365,7 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3520,7 +4373,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3528,7 +4381,7 @@
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3536,7 +4389,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3544,7 +4397,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3552,7 +4405,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3560,7 +4413,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3568,7 +4421,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3576,7 +4429,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3584,7 +4437,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3592,7 +4445,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3600,7 +4453,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3608,7 +4461,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3616,7 +4469,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3624,7 +4477,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3632,7 +4485,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3640,7 +4493,7 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3648,7 +4501,7 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3656,7 +4509,7 @@
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3664,7 +4517,7 @@
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="4">
-        <f>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</f>
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3673,45 +4526,45 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6">
-        <f>HOUR(SUM(Table24[time_diff]))*3600 + MINUTE(SUM(Table24[time_diff])) * 60 + SECOND(SUM(Table24[time_diff]))</f>
-        <v>60</v>
+        <f>HOUR(SUM(Table24511[time_diff]))*3600 + MINUTE(SUM(Table24511[time_diff])) * 60 + SECOND(SUM(Table24511[time_diff]))</f>
+        <v>2043</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5">
-        <v>0.37847222222222221</v>
+        <v>0.46736111111111112</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
-        <v>0.62847222222222221</v>
+        <v>0.61597222222222225</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>21600</v>
+        <v>12840</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E37" s="6"/>
     </row>
@@ -3727,6 +4580,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF6C17F5D6D98C42BF7485206F8FA016" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5edc83b350af0a5b53db876fcbb948f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3322fca5-43da-49d1-b081-466ee88b9b9d" xmlns:ns3="08edd21d-9f77-405a-872a-1371c16ee465" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af4f449426634c4d4ecdf601b9961ca0" ns2:_="" ns3:_="">
     <xsd:import namespace="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
@@ -3961,27 +4834,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3998,29 +4876,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
We reviewed raw footage and there was an error with VCAS-010 data. The data has been correcrted and is now reflected.
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-I-rove_time.xlsx
+++ b/data/raw/VCAS-I-rove_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75A45FF-A20F-484F-BBAD-697EA6F95F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EA7E26-C2E6-214C-80DC-3EABCC0E7272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20720" windowHeight="19960" activeTab="7" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet name="1-001" sheetId="10" r:id="rId3"/>
     <sheet name="1-002" sheetId="13" r:id="rId4"/>
     <sheet name="1-005" sheetId="14" r:id="rId5"/>
-    <sheet name="1-010" sheetId="15" r:id="rId6"/>
-    <sheet name="1-012" sheetId="17" r:id="rId7"/>
-    <sheet name="1-013" sheetId="16" r:id="rId8"/>
-    <sheet name="1-014" sheetId="19" r:id="rId9"/>
-    <sheet name="1-015" sheetId="18" r:id="rId10"/>
-    <sheet name="template" sheetId="11" r:id="rId11"/>
+    <sheet name="1-010-original" sheetId="20" r:id="rId6"/>
+    <sheet name="1-010" sheetId="15" r:id="rId7"/>
+    <sheet name="1-012" sheetId="17" r:id="rId8"/>
+    <sheet name="1-013" sheetId="16" r:id="rId9"/>
+    <sheet name="1-014" sheetId="19" r:id="rId10"/>
+    <sheet name="1-015" sheetId="18" r:id="rId11"/>
+    <sheet name="template" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,8 +46,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7BE208D0-42FA-2B4E-851E-C34653FDA30D}</author>
+    <author>tc={B84037D4-0D94-FF45-A18E-2604E7D7E883}</author>
+  </authors>
+  <commentList>
+    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{7BE208D0-42FA-2B4E-851E-C34653FDA30D}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    At the start of the video, we already have an agilis in. </t>
+      </text>
+    </comment>
+    <comment ref="C36" authorId="1" shapeId="0" xr:uid="{B84037D4-0D94-FF45-A18E-2604E7D7E883}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is time on the Pruka when skin closure happened on the camera files. We still don’t have access time. </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="88">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -226,9 +254,6 @@
   </si>
   <si>
     <t>60s rule: If a physician gets distracted with something other than ablate/move for more than 60s</t>
-  </si>
-  <si>
-    <t>What do we do if are lesion sets are broken up? Aka, what do we do if we “stop” the timer? : A timer always “starts” when the first application is delivered and ends with the last, time repositioning is not included.</t>
   </si>
   <si>
     <r>
@@ -424,6 +449,21 @@
   </si>
   <si>
     <t>map and term during VT2</t>
+  </si>
+  <si>
+    <t>What do we do if are lesion sets are broken up? Aka, what do we do if we “stop” the timer? : A timer always “starts” when the first application is delivered and ends with the last, time repositioning back into place if they moved is not included.</t>
+  </si>
+  <si>
+    <t>This is the end of mix_1, video resumes on mix_2</t>
+  </si>
+  <si>
+    <t>Stopped to map VT</t>
+  </si>
+  <si>
+    <t>VT reinduced at 12:52:30</t>
+  </si>
+  <si>
+    <t>This was the sheet submitted with initial VT efficiency metrics</t>
   </si>
 </sst>
 </file>
@@ -506,7 +546,16 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
     </dxf>
@@ -613,16 +662,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jonathan Salas" id="{7CE89E93-A593-184B-AE21-F9C35D91EED4}" userId="S::jsalas@fieldmedicalinc.com::2dbcc1de-7ea7-4748-93b5-b1d4063d54fe" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:G33" totalsRowShown="0">
   <autoFilter ref="A1:G33" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="28"/>
     <tableColumn id="3" xr3:uid="{A7F69E93-3952-2D4F-B01B-B9EB9DC3432C}" name="link_to_data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -630,12 +685,27 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{039AD6AB-0126-1947-A333-DE36DDA0B7E4}" name="Table245" displayName="Table245" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="6">
+      <calculatedColumnFormula>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F8493A5C-0C25-FD45-A552-FE369F4F3DAD}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}" name="Table24" displayName="Table24" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="3">
       <calculatedColumnFormula>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{5466BD7A-7146-7E49-B844-B14DB335F671}" name="notes"/>
@@ -650,7 +720,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{01F56379-480D-E144-8844-79E29F338160}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{80A1EC3F-97BF-2A42-A823-A672AD58C802}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="27">
       <calculatedColumnFormula>Table2[[#This Row],[end_time]]-Table2[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DC0F7FFE-563B-3E40-AAB4-A68B98253F92}" name="notes"/>
@@ -663,9 +733,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAC55445-B449-1B46-ADAD-5D1EE6A1BD3D}" name="Table246" displayName="Table246" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="24">
       <calculatedColumnFormula>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{838825F0-239B-C440-9C0B-3A9D1E9C0D95}" name="notes"/>
@@ -678,9 +748,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7DEA103-B67A-0B49-99E5-BEE70970D4BB}" name="Table247" displayName="Table247" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="21">
       <calculatedColumnFormula>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{CCA0740F-5707-C44E-AA57-B44DAE132805}" name="notes"/>
@@ -690,12 +760,27 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F5A4CEBC-9F74-3B4A-97EE-FBFC2B092D3F}" name="Table24812" displayName="Table24812" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="0">
+      <calculatedColumnFormula>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F0480389-BE2E-CA47-91C9-281947E722D0}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{772A68B7-3577-954E-96AB-3F9F135762FE}" name="Table248" displayName="Table248" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="18">
       <calculatedColumnFormula>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F22060DE-01C3-9C4C-A473-BCE8D37580D6}" name="notes"/>
@@ -704,13 +789,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D84B3EF0-7875-184B-870A-3642242A31F0}" name="Table2410" displayName="Table2410" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="15">
       <calculatedColumnFormula>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7A57ED91-2446-8F4F-95C2-3088CD96BD62}" name="notes"/>
@@ -719,13 +804,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A3CEC53-F376-1D4D-846C-0F34B09239B4}" name="Table249" displayName="Table249" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="12">
       <calculatedColumnFormula>Table249[[#This Row],[end_time]]-Table249[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7880A518-97D3-0D44-977A-E75D9468AB4A}" name="notes"/>
@@ -734,31 +819,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A7ADDBBE-0483-F84D-98C5-791E3CFC3CE4}" name="Table24511" displayName="Table24511" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="9">
       <calculatedColumnFormula>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{6BF25E36-BEFE-334C-B53B-9359DA68008A}" name="notes"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{039AD6AB-0126-1947-A333-DE36DDA0B7E4}" name="Table245" displayName="Table245" ref="A1:D31" totalsRowShown="0">
-  <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="3">
-      <calculatedColumnFormula>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{F8493A5C-0C25-FD45-A552-FE369F4F3DAD}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1079,12 +1149,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C35" dT="2024-08-08T17:12:18.97" personId="{7CE89E93-A593-184B-AE21-F9C35D91EED4}" id="{7BE208D0-42FA-2B4E-851E-C34653FDA30D}">
+    <text xml:space="preserve">At the start of the video, we already have an agilis in. </text>
+  </threadedComment>
+  <threadedComment ref="C36" dT="2024-08-08T17:12:07.01" personId="{7CE89E93-A593-184B-AE21-F9C35D91EED4}" id="{B84037D4-0D94-FF45-A18E-2604E7D7E883}">
+    <text xml:space="preserve">This is time on the Pruka when skin closure happened on the camera files. We still don’t have access time. </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535426F-7A8C-E949-810F-FB71A9FDBD02}">
   <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView zoomScale="179" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A10" zoomScale="161" workbookViewId="0">
+      <selection activeCell="A35" sqref="A17:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,37 +1242,37 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1200,6 +1281,358 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E96B43-315A-A34D-AC7F-DA126C47C92D}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>0.55614583333333334</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.56443287037037038</v>
+      </c>
+      <c r="C2" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>8.2870370370370372E-3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>0.57165509259259262</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.57843750000000005</v>
+      </c>
+      <c r="C3" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>6.7824074074074314E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>0.58763888888888893</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.59467592592592589</v>
+      </c>
+      <c r="C4" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>7.0370370370369528E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>0.60098379629629628</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.60252314814814811</v>
+      </c>
+      <c r="C5" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>1.5393518518518334E-3</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4">
+        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="6">
+        <f>HOUR(SUM(Table24511[time_diff]))*3600 + MINUTE(SUM(Table24511[time_diff])) * 60 + SECOND(SUM(Table24511[time_diff]))</f>
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.46736111111111112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.61597222222222225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6">
+        <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
+        <v>12840</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88A8D6D-D290-9244-9467-AD71E2C0964F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
@@ -1530,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5D0936-41CB-4D48-9AD9-6C4AF0186848}">
   <dimension ref="A1:G41"/>
   <sheetViews>
@@ -1865,8 +2298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1892,7 +2325,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
@@ -1915,7 +2348,7 @@
         <v>77</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>17</v>
@@ -1938,7 +2371,7 @@
         <v>165</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="3" t="s">
@@ -1956,13 +2389,13 @@
         <v>95</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1973,14 +2406,13 @@
         <v>17760</v>
       </c>
       <c r="C5" s="6">
-        <f>HOUR(SUM(Table248[time_diff]))*3600 + MINUTE(SUM(Table248[time_diff])) * 60 + SECOND(SUM(Table248[time_diff]))</f>
-        <v>542</v>
+        <v>1993</v>
       </c>
       <c r="D5" s="6">
         <v>75</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
@@ -2012,7 +2444,7 @@
         <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="8" t="s">
@@ -2033,18 +2465,18 @@
         <v>31</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="6">
         <v>12840</v>
@@ -2056,16 +2488,16 @@
         <v>105</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="6">
         <v>9600</v>
@@ -2077,11 +2509,11 @@
         <v>35</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2865,7 +3297,690 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F32F5E9-1E20-D04B-A430-E1A4492E325E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F32F5E9-1E20-D04B-A430-E1A4492E325E}">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>0.64217592592592587</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.65585648148148146</v>
+      </c>
+      <c r="C2" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>1.3680555555555585E-2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.67078703703703701</v>
+      </c>
+      <c r="C3" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>1.3425925925926174E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>0.68248842592592596</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.68859953703703702</v>
+      </c>
+      <c r="C4" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>6.1111111111110672E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>3.8310185185185183E-3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>6.7129629629629631E-3</v>
+      </c>
+      <c r="C5" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>2.8819444444444448E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4">
+        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="6">
+        <f>HOUR(SUM(Table247[time_diff]))*3600 + MINUTE(SUM(Table247[time_diff])) * 60 + SECOND(SUM(Table247[time_diff]))</f>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.21180555555555555</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6">
+        <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
+        <v>18300</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38E92CE-29F7-6D4F-BC97-A709947D3371}">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>2.1956018518518517E-2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2.4641203703703703E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>2.6851851851851863E-3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>5.7141203703703701E-2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5.752314814814815E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>3.8194444444444864E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>7.5046296296296292E-2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>7.8252314814814816E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>3.2060185185185247E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4">
+        <f>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="6">
+        <f>HOUR(SUM(Table24812[time_diff]))*3600 + MINUTE(SUM(Table24812[time_diff])) * 60 + SECOND(SUM(Table24812[time_diff]))</f>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.36527777777777776</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.5708333333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6">
+        <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
+        <v>17760</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586AB6B7-C4D5-5842-A12D-7C2673B4EDD7}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2893,77 +4008,78 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>0.64217592592592587</v>
+        <v>0.49760416666666668</v>
       </c>
       <c r="B2" s="5">
-        <v>0.65585648148148146</v>
+        <v>0.50002314814814819</v>
       </c>
       <c r="C2" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>1.3680555555555585E-2</v>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <v>2.418981481481508E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>0.6694444444444444</v>
+        <v>0.50552083333333331</v>
       </c>
       <c r="B3" s="5">
-        <v>0.67078703703703701</v>
+        <v>0.5119097222222222</v>
       </c>
       <c r="C3" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>1.3425925925926174E-3</v>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <v>6.3888888888888884E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>0.68248842592592596</v>
+        <v>0.5119097222222222</v>
       </c>
       <c r="B4" s="5">
-        <v>0.68859953703703702</v>
+        <v>0.52406249999999999</v>
       </c>
       <c r="C4" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>6.1111111111110672E-3</v>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <v>1.215277777777779E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>3.8310185185185183E-3</v>
+        <v>0.53478009259259263</v>
       </c>
       <c r="B5" s="5">
-        <v>6.7129629629629631E-3</v>
+        <v>0.53651620370370368</v>
       </c>
       <c r="C5" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>2.8819444444444448E-3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <v>1.7361111111110494E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="5">
+        <v>0.56906250000000003</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.56943287037037038</v>
+      </c>
       <c r="C6" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <v>3.7037037037035425E-4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -2971,7 +4087,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -2979,7 +4095,7 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -2987,7 +4103,7 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -2995,7 +4111,7 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3003,7 +4119,7 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3011,7 +4127,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3019,7 +4135,7 @@
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3027,7 +4143,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3035,7 +4151,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3043,7 +4159,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3051,7 +4167,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3059,7 +4175,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3067,7 +4183,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3075,7 +4191,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3083,7 +4199,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3091,7 +4207,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3099,7 +4215,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3107,7 +4223,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3115,7 +4231,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3123,7 +4239,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3131,7 +4247,7 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3139,7 +4255,7 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3147,7 +4263,7 @@
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3155,7 +4271,7 @@
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="4">
-        <f>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</f>
+        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3164,8 +4280,8 @@
         <v>56</v>
       </c>
       <c r="C33" s="6">
-        <f>HOUR(SUM(Table247[time_diff]))*3600 + MINUTE(SUM(Table247[time_diff])) * 60 + SECOND(SUM(Table247[time_diff]))</f>
-        <v>2075</v>
+        <f>HOUR(SUM(Table248[time_diff]))*3600 + MINUTE(SUM(Table248[time_diff])) * 60 + SECOND(SUM(Table248[time_diff]))</f>
+        <v>1993</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3179,7 +4295,7 @@
         <v>47</v>
       </c>
       <c r="C35" s="5">
-        <v>0</v>
+        <v>0.36527777777777776</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3187,7 +4303,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <v>0</v>
+        <v>0.5708333333333333</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3196,7 +4312,7 @@
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>0</v>
+        <v>17760</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
@@ -3210,11 +4326,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586AB6B7-C4D5-5842-A12D-7C2673B4EDD7}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE23BA92-9E5F-3D40-BA9A-5D51FC245316}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -3239,56 +4355,69 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>2.1956018518518517E-2</v>
+        <v>4.6053240740740742E-2</v>
       </c>
       <c r="B2" s="5">
-        <v>2.4641203703703703E-2</v>
+        <v>5.6851851851851855E-2</v>
       </c>
       <c r="C2" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
-        <v>2.6851851851851863E-3</v>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
+        <v>1.0798611111111113E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>5.7141203703703701E-2</v>
+        <v>5.966435185185185E-2</v>
       </c>
       <c r="B3" s="5">
-        <v>5.752314814814815E-2</v>
+        <v>6.7222222222222225E-2</v>
       </c>
       <c r="C3" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
-        <v>3.8194444444444864E-4</v>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
+        <v>7.5578703703703745E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>7.5046296296296292E-2</v>
+        <v>7.4062500000000003E-2</v>
       </c>
       <c r="B4" s="5">
-        <v>7.8252314814814816E-2</v>
+        <v>7.5462962962962968E-2</v>
       </c>
       <c r="C4" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
-        <v>3.2060185185185247E-3</v>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
+        <v>1.4004629629629645E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="5">
+        <v>8.548611111111111E-2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>8.5798611111111117E-2</v>
+      </c>
       <c r="C5" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
-        <v>0</v>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
+        <v>3.1250000000000722E-4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3296,7 +4425,7 @@
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3304,7 +4433,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3312,7 +4441,7 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3320,7 +4449,7 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3328,7 +4457,7 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3336,7 +4465,7 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3344,7 +4473,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3352,7 +4481,7 @@
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3360,7 +4489,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3368,7 +4497,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3376,7 +4505,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3384,7 +4513,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3392,7 +4521,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3400,7 +4529,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3408,7 +4537,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3416,7 +4545,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3424,7 +4553,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3432,7 +4561,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3440,7 +4569,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3448,7 +4577,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3456,7 +4585,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3464,7 +4593,7 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3472,7 +4601,7 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3480,7 +4609,7 @@
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3488,7 +4617,7 @@
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="4">
-        <f>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</f>
+        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3497,8 +4626,8 @@
         <v>56</v>
       </c>
       <c r="C33" s="6">
-        <f>HOUR(SUM(Table248[time_diff]))*3600 + MINUTE(SUM(Table248[time_diff])) * 60 + SECOND(SUM(Table248[time_diff]))</f>
-        <v>542</v>
+        <f>HOUR(SUM(Table2410[time_diff]))*3600 + MINUTE(SUM(Table2410[time_diff])) * 60 + SECOND(SUM(Table2410[time_diff]))</f>
+        <v>1734</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3512,7 +4641,7 @@
         <v>47</v>
       </c>
       <c r="C35" s="5">
-        <v>0.36527777777777776</v>
+        <v>0.44583333333333336</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3520,7 +4649,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <v>0.5708333333333333</v>
+        <v>0.54861111111111116</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3529,7 +4658,7 @@
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>17760</v>
+        <v>8880</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
@@ -3543,353 +4672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE23BA92-9E5F-3D40-BA9A-5D51FC245316}">
-  <dimension ref="A1:D37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="72.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>4.6053240740740742E-2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>5.6851851851851855E-2</v>
-      </c>
-      <c r="C2" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>1.0798611111111113E-2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>5.966435185185185E-2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>6.7222222222222225E-2</v>
-      </c>
-      <c r="C3" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>7.5578703703703745E-3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>7.4062500000000003E-2</v>
-      </c>
-      <c r="B4" s="5">
-        <v>7.5462962962962968E-2</v>
-      </c>
-      <c r="C4" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>1.4004629629629645E-3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>8.548611111111111E-2</v>
-      </c>
-      <c r="B5" s="5">
-        <v>8.5798611111111117E-2</v>
-      </c>
-      <c r="C5" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>3.1250000000000722E-4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4">
-        <f>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="6">
-        <f>HOUR(SUM(Table2410[time_diff]))*3600 + MINUTE(SUM(Table2410[time_diff])) * 60 + SECOND(SUM(Table2410[time_diff]))</f>
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="5">
-        <v>0.44583333333333336</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="5">
-        <v>0.54861111111111116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="6">
-        <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>8880</v>
-      </c>
-      <c r="D37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A2C8FE-39BB-BB4A-8DDF-4FBE8810A41F}">
   <dimension ref="A1:D37"/>
   <sheetViews>
@@ -4227,379 +5010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E96B43-315A-A34D-AC7F-DA126C47C92D}">
-  <dimension ref="A1:G41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="72.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>0.55614583333333334</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0.56443287037037038</v>
-      </c>
-      <c r="C2" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>8.2870370370370372E-3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>0.57165509259259262</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.57843750000000005</v>
-      </c>
-      <c r="C3" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>6.7824074074074314E-3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>0.58763888888888893</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0.59467592592592589</v>
-      </c>
-      <c r="C4" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>7.0370370370369528E-3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>0.60098379629629628</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.60252314814814811</v>
-      </c>
-      <c r="C5" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>1.5393518518518334E-3</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4">
-        <f>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="6">
-        <f>HOUR(SUM(Table24511[time_diff]))*3600 + MINUTE(SUM(Table24511[time_diff])) * 60 + SECOND(SUM(Table24511[time_diff]))</f>
-        <v>2043</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="5">
-        <v>0.46736111111111112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="5">
-        <v>0.61597222222222225</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="6">
-        <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>12840</v>
-      </c>
-      <c r="D37" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D41" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF6C17F5D6D98C42BF7485206F8FA016" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5edc83b350af0a5b53db876fcbb948f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3322fca5-43da-49d1-b081-466ee88b9b9d" xmlns:ns3="08edd21d-9f77-405a-872a-1371c16ee465" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af4f449426634c4d4ecdf601b9961ca0" ns2:_="" ns3:_="">
     <xsd:import namespace="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
@@ -4834,10 +5245,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
+    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4860,20 +5302,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
-    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
VCAS-002 ablation and procedure time were just wrong.
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-I-rove_time.xlsx
+++ b/data/raw/VCAS-I-rove_time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EA7E26-C2E6-214C-80DC-3EABCC0E7272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED45FA57-0C44-8C4F-994F-91637CCD0D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="20720" windowHeight="19960" activeTab="7" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="12600" yWindow="760" windowWidth="25280" windowHeight="19880" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="1-001" sheetId="10" r:id="rId3"/>
     <sheet name="1-002" sheetId="13" r:id="rId4"/>
     <sheet name="1-005" sheetId="14" r:id="rId5"/>
-    <sheet name="1-010-original" sheetId="20" r:id="rId6"/>
+    <sheet name="1-010-original" sheetId="20" state="hidden" r:id="rId6"/>
     <sheet name="1-010" sheetId="15" r:id="rId7"/>
     <sheet name="1-012" sheetId="17" r:id="rId8"/>
     <sheet name="1-013" sheetId="16" r:id="rId9"/>
@@ -51,6 +51,7 @@
   <authors>
     <author>tc={7BE208D0-42FA-2B4E-851E-C34653FDA30D}</author>
     <author>tc={B84037D4-0D94-FF45-A18E-2604E7D7E883}</author>
+    <author>tc={3256EE5F-4B7B-4A4B-94EB-63488F43CEF4}</author>
   </authors>
   <commentList>
     <comment ref="C35" authorId="0" shapeId="0" xr:uid="{7BE208D0-42FA-2B4E-851E-C34653FDA30D}">
@@ -69,12 +70,20 @@
     This is time on the Pruka when skin closure happened on the camera files. We still don’t have access time. </t>
       </text>
     </comment>
+    <comment ref="C37" authorId="2" shapeId="0" xr:uid="{3256EE5F-4B7B-4A4B-94EB-63488F43CEF4}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Wrong, don’t use this value. </t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="92">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -465,6 +474,18 @@
   <si>
     <t>This was the sheet submitted with initial VT efficiency metrics</t>
   </si>
+  <si>
+    <t>induced VT with abl - attemped to term with ATP then abl, it failed. CVN at 2:20:04</t>
+  </si>
+  <si>
+    <t>Induced VT with abl - 2:22:59, didn't term. Stop to troubleshoot CARTO</t>
+  </si>
+  <si>
+    <t>stop to troubleshoot catheter</t>
+  </si>
+  <si>
+    <t>In first version, we left out the first 3 sets of lesions</t>
+  </si>
 </sst>
 </file>
 
@@ -473,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -501,6 +522,13 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -530,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -541,6 +569,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -688,9 +717,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{039AD6AB-0126-1947-A333-DE36DDA0B7E4}" name="Table245" displayName="Table245" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="3">
       <calculatedColumnFormula>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F8493A5C-0C25-FD45-A552-FE369F4F3DAD}" name="notes"/>
@@ -703,9 +732,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}" name="Table24" displayName="Table24" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="0">
       <calculatedColumnFormula>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{5466BD7A-7146-7E49-B844-B14DB335F671}" name="notes"/>
@@ -763,9 +792,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F5A4CEBC-9F74-3B4A-97EE-FBFC2B092D3F}" name="Table24812" displayName="Table24812" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="18">
       <calculatedColumnFormula>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F0480389-BE2E-CA47-91C9-281947E722D0}" name="notes"/>
@@ -778,9 +807,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{772A68B7-3577-954E-96AB-3F9F135762FE}" name="Table248" displayName="Table248" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="15">
       <calculatedColumnFormula>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F22060DE-01C3-9C4C-A473-BCE8D37580D6}" name="notes"/>
@@ -793,9 +822,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D84B3EF0-7875-184B-870A-3642242A31F0}" name="Table2410" displayName="Table2410" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="12">
       <calculatedColumnFormula>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7A57ED91-2446-8F4F-95C2-3088CD96BD62}" name="notes"/>
@@ -808,9 +837,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A3CEC53-F376-1D4D-846C-0F34B09239B4}" name="Table249" displayName="Table249" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="9">
       <calculatedColumnFormula>Table249[[#This Row],[end_time]]-Table249[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7880A518-97D3-0D44-977A-E75D9468AB4A}" name="notes"/>
@@ -823,9 +852,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A7ADDBBE-0483-F84D-98C5-791E3CFC3CE4}" name="Table24511" displayName="Table24511" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="6">
       <calculatedColumnFormula>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{6BF25E36-BEFE-334C-B53B-9359DA68008A}" name="notes"/>
@@ -1157,6 +1186,9 @@
   <threadedComment ref="C36" dT="2024-08-08T17:12:07.01" personId="{7CE89E93-A593-184B-AE21-F9C35D91EED4}" id="{B84037D4-0D94-FF45-A18E-2604E7D7E883}">
     <text xml:space="preserve">This is time on the Pruka when skin closure happened on the camera files. We still don’t have access time. </text>
   </threadedComment>
+  <threadedComment ref="C37" dT="2024-08-15T21:24:05.53" personId="{7CE89E93-A593-184B-AE21-F9C35D91EED4}" id="{3256EE5F-4B7B-4A4B-94EB-63488F43CEF4}">
+    <text xml:space="preserve">Wrong, don’t use this value. </text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2298,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2362,10 +2394,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="6">
-        <v>5640</v>
+        <v>15000</v>
       </c>
       <c r="C3" s="6">
-        <v>3025</v>
+        <v>3965</v>
       </c>
       <c r="D3" s="6">
         <v>165</v>
@@ -2945,10 +2977,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F9F9B0-7F62-0F40-BBEB-48DA30804DB0}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A6" zoomScale="131" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2956,7 +2988,7 @@
     <col min="4" max="4" width="72.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2970,106 +3002,130 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>0.11532407407407408</v>
+        <v>9.4745370370370369E-2</v>
       </c>
       <c r="B2" s="5">
-        <v>0.11841435185185185</v>
+        <v>9.6180555555555561E-2</v>
       </c>
       <c r="C2" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>3.0902777777777751E-3</v>
+        <v>1.4351851851851921E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>0.11849537037037038</v>
+        <v>9.8032407407407401E-2</v>
       </c>
       <c r="B3" s="5">
-        <v>0.12291666666666666</v>
+        <v>0.10219907407407407</v>
       </c>
       <c r="C3" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>4.4212962962962843E-3</v>
+        <v>4.1666666666666657E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>0.12600694444444444</v>
+        <v>0.10553240740740741</v>
       </c>
       <c r="B4" s="5">
-        <v>0.15243055555555557</v>
+        <v>0.11081018518518519</v>
       </c>
       <c r="C4" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>2.6423611111111134E-2</v>
+        <v>5.277777777777784E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>0.16231481481481483</v>
+        <v>0.11532407407407408</v>
       </c>
       <c r="B5" s="5">
-        <v>0.16296296296296298</v>
+        <v>0.11841435185185185</v>
       </c>
       <c r="C5" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>6.481481481481477E-4</v>
+        <v>3.0902777777777751E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>0.1713888888888889</v>
+        <v>0.11849537037037038</v>
       </c>
       <c r="B6" s="5">
-        <v>0.17181712962962964</v>
+        <v>0.12291666666666666</v>
       </c>
       <c r="C6" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>4.2824074074074292E-4</v>
+        <v>4.4212962962962843E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>0.12600694444444444</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.15243055555555557</v>
+      </c>
       <c r="C7" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+        <v>2.6423611111111134E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>0.16231481481481483</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.16296296296296298</v>
+      </c>
       <c r="C8" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+        <v>6.481481481481477E-4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>0.1713888888888889</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.17181712962962964</v>
+      </c>
       <c r="C9" s="4">
         <f>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4.2824074074074292E-4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4">
@@ -3077,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4">
@@ -3085,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4">
@@ -3093,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4">
@@ -3101,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4">
@@ -3109,7 +3165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="4">
@@ -3117,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4">
@@ -3251,7 +3307,7 @@
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table246[time_diff]))*3600 + MINUTE(SUM(Table246[time_diff])) * 60 + SECOND(SUM(Table246[time_diff]))</f>
-        <v>3025</v>
+        <v>3965</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3265,7 +3321,7 @@
         <v>47</v>
       </c>
       <c r="C35" s="5">
-        <v>0.40277777777777779</v>
+        <v>0.37847222222222221</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3273,7 +3329,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <v>0.46805555555555556</v>
+        <v>0.55208333333333337</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3282,7 +3338,7 @@
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>5640</v>
+        <v>15000</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
@@ -3301,7 +3357,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3626,7 +3682,7 @@
       <c r="A37" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="10">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
         <v>18300</v>
       </c>
@@ -4330,7 +4386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE23BA92-9E5F-3D40-BA9A-5D51FC245316}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -5011,6 +5067,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF6C17F5D6D98C42BF7485206F8FA016" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5edc83b350af0a5b53db876fcbb948f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3322fca5-43da-49d1-b081-466ee88b9b9d" xmlns:ns3="08edd21d-9f77-405a-872a-1371c16ee465" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af4f449426634c4d4ecdf601b9961ca0" ns2:_="" ns3:_="">
     <xsd:import namespace="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
@@ -5245,41 +5321,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
-    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5302,9 +5347,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
+    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
I hate you and the typos you make. Fixed procedure times for VCAS-02 as well.
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-I-rove_time.xlsx
+++ b/data/raw/VCAS-I-rove_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED45FA57-0C44-8C4F-994F-91637CCD0D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A86081-9BFC-EB41-B1BB-FC05517FA370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="760" windowWidth="25280" windowHeight="19880" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="17300" yWindow="760" windowWidth="17260" windowHeight="19880" firstSheet="2" activeTab="11" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -1316,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E96B43-315A-A34D-AC7F-DA126C47C92D}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="106" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -1999,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5D0936-41CB-4D48-9AD9-6C4AF0186848}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2330,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2394,7 +2394,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="6">
-        <v>15000</v>
+        <v>17100</v>
       </c>
       <c r="C3" s="6">
         <v>3965</v>
@@ -2666,7 +2666,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2980,7 +2980,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="131" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3329,7 +3329,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <v>0.55208333333333337</v>
+        <v>0.57638888888888884</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>15000</v>
+        <v>17100</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
@@ -4386,7 +4386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE23BA92-9E5F-3D40-BA9A-5D51FC245316}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="125" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -4732,7 +4732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A2C8FE-39BB-BB4A-8DDF-4FBE8810A41F}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="125" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -5067,26 +5067,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF6C17F5D6D98C42BF7485206F8FA016" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5edc83b350af0a5b53db876fcbb948f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3322fca5-43da-49d1-b081-466ee88b9b9d" xmlns:ns3="08edd21d-9f77-405a-872a-1371c16ee465" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af4f449426634c4d4ecdf601b9961ca0" ns2:_="" ns3:_="">
     <xsd:import namespace="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
@@ -5321,10 +5301,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
+    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5347,20 +5358,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10E5675-4834-416E-A2AA-AFEE37EB2CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
-    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update raw data to include dwell time
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-I-rove_time.xlsx
+++ b/data/raw/VCAS-I-rove_time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BD444B-1E58-824A-9B9B-D406ED61B600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A69525F-76B0-644A-B59D-10335C5DD412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17300" yWindow="760" windowWidth="17260" windowHeight="19880" firstSheet="2" activeTab="7" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="98">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -486,6 +486,24 @@
   <si>
     <t>In first version, we left out the first 3 sets of lesions</t>
   </si>
+  <si>
+    <t>dwell_time</t>
+  </si>
+  <si>
+    <t>Total Dwell Time = Catheter Out - Catheter In</t>
+  </si>
+  <si>
+    <t>Catheter Out</t>
+  </si>
+  <si>
+    <t>Catheter In</t>
+  </si>
+  <si>
+    <t>Total Dwell Time</t>
+  </si>
+  <si>
+    <t>dwell_time is expressed in seconds. It is fieldforce out minus fieldforce in</t>
+  </si>
 </sst>
 </file>
 
@@ -494,7 +512,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -530,6 +548,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -558,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -570,12 +595,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="35">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
     </dxf>
@@ -698,15 +728,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:G33" totalsRowShown="0">
-  <autoFilter ref="A1:G33" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:H33" totalsRowShown="0">
+  <autoFilter ref="A1:H33" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{5E0CEC32-C01F-A446-827E-6309FE417F82}" name="dwell_time" dataDxfId="0">
+      <calculatedColumnFormula>'1-001'!C41</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="29"/>
     <tableColumn id="3" xr3:uid="{A7F69E93-3952-2D4F-B01B-B9EB9DC3432C}" name="link_to_data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -717,9 +750,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{039AD6AB-0126-1947-A333-DE36DDA0B7E4}" name="Table245" displayName="Table245" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="4">
       <calculatedColumnFormula>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F8493A5C-0C25-FD45-A552-FE369F4F3DAD}" name="notes"/>
@@ -732,9 +765,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}" name="Table24" displayName="Table24" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{90F3E024-3E74-4A41-BA3F-E0CAE2A1648D}" name="start_time" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{57A35EB3-231B-FD48-B4FC-CE8C47535B43}" name="end_time" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{21ACA455-5123-234C-B7BB-9A75B83EFDE5}" name="time_diff" dataDxfId="1">
       <calculatedColumnFormula>Table24[[#This Row],[end_time]]-Table24[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{5466BD7A-7146-7E49-B844-B14DB335F671}" name="notes"/>
@@ -749,7 +782,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{01F56379-480D-E144-8844-79E29F338160}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{80A1EC3F-97BF-2A42-A823-A672AD58C802}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="27">
+    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="28">
       <calculatedColumnFormula>Table2[[#This Row],[end_time]]-Table2[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DC0F7FFE-563B-3E40-AAB4-A68B98253F92}" name="notes"/>
@@ -762,9 +795,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAC55445-B449-1B46-ADAD-5D1EE6A1BD3D}" name="Table246" displayName="Table246" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="25">
       <calculatedColumnFormula>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{838825F0-239B-C440-9C0B-3A9D1E9C0D95}" name="notes"/>
@@ -777,9 +810,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7DEA103-B67A-0B49-99E5-BEE70970D4BB}" name="Table247" displayName="Table247" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="22">
       <calculatedColumnFormula>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{CCA0740F-5707-C44E-AA57-B44DAE132805}" name="notes"/>
@@ -792,9 +825,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F5A4CEBC-9F74-3B4A-97EE-FBFC2B092D3F}" name="Table24812" displayName="Table24812" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="19">
       <calculatedColumnFormula>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F0480389-BE2E-CA47-91C9-281947E722D0}" name="notes"/>
@@ -807,9 +840,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{772A68B7-3577-954E-96AB-3F9F135762FE}" name="Table248" displayName="Table248" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="16">
       <calculatedColumnFormula>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F22060DE-01C3-9C4C-A473-BCE8D37580D6}" name="notes"/>
@@ -822,9 +855,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D84B3EF0-7875-184B-870A-3642242A31F0}" name="Table2410" displayName="Table2410" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="13">
       <calculatedColumnFormula>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7A57ED91-2446-8F4F-95C2-3088CD96BD62}" name="notes"/>
@@ -837,9 +870,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A3CEC53-F376-1D4D-846C-0F34B09239B4}" name="Table249" displayName="Table249" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="10">
       <calculatedColumnFormula>Table249[[#This Row],[end_time]]-Table249[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7880A518-97D3-0D44-977A-E75D9468AB4A}" name="notes"/>
@@ -852,9 +885,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A7ADDBBE-0483-F84D-98C5-791E3CFC3CE4}" name="Table24511" displayName="Table24511" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="7">
       <calculatedColumnFormula>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{6BF25E36-BEFE-334C-B53B-9359DA68008A}" name="notes"/>
@@ -1194,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535426F-7A8C-E949-810F-FB71A9FDBD02}">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="161" workbookViewId="0">
-      <selection activeCell="A35" sqref="A17:A35"/>
+    <sheetView zoomScale="161" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,56 +1287,61 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1314,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E96B43-315A-A34D-AC7F-DA126C47C92D}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1653,8 +1691,41 @@
       </c>
       <c r="E37" s="6"/>
     </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12">
+        <v>0.63611111111111107</v>
+      </c>
+    </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12">
+        <v>0.68611111111111112</v>
+      </c>
       <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>4320</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1666,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88A8D6D-D290-9244-9467-AD71E2C0964F}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1984,8 +2055,41 @@
       </c>
       <c r="E37" s="6"/>
     </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12">
+        <v>0.78472222222222221</v>
+      </c>
       <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>1200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2328,22 +2432,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="53.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="3" max="5" width="11.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="53.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2357,16 +2461,19 @@
         <v>52</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2379,17 +2486,21 @@
       <c r="D2" s="6">
         <v>77</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="6">
+        <f>'1-001'!C42</f>
+        <v>13680</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2402,15 +2513,19 @@
       <c r="D3" s="6">
         <v>165</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="6">
+        <f>'1-002'!C42</f>
+        <v>5520</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2420,17 +2535,21 @@
       <c r="D4" s="6">
         <v>95</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="6">
+        <f>'1-005'!C42</f>
+        <v>6660</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2443,26 +2562,30 @@
       <c r="D5" s="6">
         <v>75</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="6">
+        <f>'1-010'!C42</f>
+        <v>8040</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2475,15 +2598,19 @@
       <c r="D7" s="6">
         <v>102</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="6">
+        <f>'1-012'!C42</f>
+        <v>3720</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -2496,17 +2623,21 @@
       <c r="D8" s="6">
         <v>31</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="6">
+        <f>'1-013'!C42</f>
+        <v>2700</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
@@ -2519,15 +2650,19 @@
       <c r="D9" s="6">
         <v>105</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="6">
+        <f>'1-014'!C42</f>
+        <v>4320</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
@@ -2540,119 +2675,215 @@
       <c r="D10" s="6">
         <v>35</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="6">
+        <f>'1-015'!C42</f>
+        <v>1200</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="6">
+        <f>'1-001'!C50</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="6">
+        <f>'1-001'!C51</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="6">
+        <f>'1-001'!C52</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="6">
+        <f>'1-001'!C53</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="6">
+        <f>'1-001'!C54</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="6">
+        <f>'1-001'!C55</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E17" s="6">
+        <f>'1-001'!C56</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E18" s="6">
+        <f>'1-001'!C57</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E19" s="6">
+        <f>'1-001'!C58</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E20" s="6">
+        <f>'1-001'!C59</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E21" s="6">
+        <f>'1-001'!C60</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E22" s="6">
+        <f>'1-001'!C61</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E23" s="6">
+        <f>'1-001'!C62</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="6">
+        <f>'1-001'!C63</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E25" s="6">
+        <f>'1-001'!C64</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E26" s="6">
+        <f>'1-001'!C65</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E27" s="6">
+        <f>'1-001'!C66</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E28" s="6">
+        <f>'1-001'!C67</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E29" s="6">
+        <f>'1-001'!C68</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E30" s="6">
+        <f>'1-001'!C69</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E31" s="6">
+        <f>'1-001'!C70</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E32" s="6">
+        <f>'1-001'!C71</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="4"/>
+      <c r="E33" s="6">
+        <f>'1-001'!C72</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
-    <hyperlink ref="G5" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
-    <hyperlink ref="G9" r:id="rId7" xr:uid="{3DBA40E2-94AD-4845-AA90-D92036F9A7B1}"/>
-    <hyperlink ref="G10" r:id="rId8" xr:uid="{53E20B43-9ECF-BE46-AB3C-B2592713D701}"/>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{3DBA40E2-94AD-4845-AA90-D92036F9A7B1}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{53E20B43-9ECF-BE46-AB3C-B2592713D701}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2663,10 +2894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31B8D96-118F-A248-83C6-FD8A563415A9}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2967,6 +3198,37 @@
         <v>51</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0.4513888888888889</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0.60972222222222228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>13680</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2977,10 +3239,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F9F9B0-7F62-0F40-BBEB-48DA30804DB0}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="131" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A15" zoomScale="131" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3344,6 +3606,37 @@
         <v>51</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0.48819444444444443</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>5520</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3354,10 +3647,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F32F5E9-1E20-D04B-A430-E1A4492E325E}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A39" sqref="A39:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3688,6 +3981,37 @@
       </c>
       <c r="D37" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0.70208333333333328</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>6660</v>
       </c>
     </row>
   </sheetData>
@@ -4037,10 +4361,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586AB6B7-C4D5-5842-A12D-7C2673B4EDD7}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4374,6 +4698,37 @@
         <v>51</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0.44305555555555554</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0.53611111111111109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>8040</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4384,10 +4739,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE23BA92-9E5F-3D40-BA9A-5D51FC245316}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4720,6 +5075,41 @@
         <v>51</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12">
+        <v>0.50069444444444444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12">
+        <v>0.54374999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>3720</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4730,10 +5120,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A2C8FE-39BB-BB4A-8DDF-4FBE8810A41F}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A39" sqref="A39:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5058,6 +5448,41 @@
         <v>51</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12">
+        <v>0.6694444444444444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12">
+        <v>0.7006944444444444</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6">
+        <f>SUM(HOUR(C41-C40)*3600 + MINUTE(C41-C40)*60 + SECOND(C41-C40))</f>
+        <v>2700</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5067,14 +5492,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5313,27 +5736,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5358,9 +5774,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="08edd21d-9f77-405a-872a-1371c16ee465"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3322fca5-43da-49d1-b081-466ee88b9b9d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added patients 16 and 17
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-I-rove_time.xlsx
+++ b/data/raw/VCAS-I-rove_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB37E12-7BB0-1247-9A67-68BA501FC269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28762C9-FECD-8E45-BCBC-3D4AC92FFFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="106">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>Huge inferior wall scar, lots of VTs</t>
+  </si>
+  <si>
+    <t>etiology</t>
+  </si>
+  <si>
+    <t>ischemic</t>
   </si>
 </sst>
 </file>
@@ -679,7 +685,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="44">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
     </dxf>
@@ -829,18 +838,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:H33" totalsRowShown="0">
-  <autoFilter ref="A1:H33" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{5E0CEC32-C01F-A446-827E-6309FE417F82}" name="dwell_time" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}" name="Table1" displayName="Table1" ref="A1:I33" totalsRowShown="0">
+  <autoFilter ref="A1:I33" xr:uid="{C55969D0-B28D-F248-8DCD-E81C0E8043BD}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="id" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{5E0CEC32-C01F-A446-827E-6309FE417F82}" name="dwell_time" dataDxfId="39">
       <calculatedColumnFormula>'1-001'!H35</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{E391ECC4-3F7C-C84F-9F85-065534605FDC}" name="etiology" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{18DD3274-05B0-9245-BC8D-9610E146E79C}" name="therapy" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{3166333D-6394-D34A-93C0-598B4DEC56B1}" name="notes" dataDxfId="37"/>
     <tableColumn id="3" xr3:uid="{A7F69E93-3952-2D4F-B01B-B9EB9DC3432C}" name="link_to_data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -851,9 +861,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A3CEC53-F376-1D4D-846C-0F34B09239B4}" name="Table249" displayName="Table249" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{49600F71-5258-BD4C-B040-17EFB93CC626}" name="start_time" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{BDE18332-AF9E-6E4E-B81F-9AB511ACDD6F}" name="end_time" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{8AAE5943-30E3-C746-AE58-07515593AE41}" name="time_diff" dataDxfId="16">
       <calculatedColumnFormula>Table249[[#This Row],[end_time]]-Table249[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7880A518-97D3-0D44-977A-E75D9468AB4A}" name="notes"/>
@@ -866,9 +876,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A7ADDBBE-0483-F84D-98C5-791E3CFC3CE4}" name="Table24511" displayName="Table24511" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{26C8DC9E-AF52-B74F-997F-91F760434CC8}" name="start_time" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6083687F-E3D1-0F47-90EE-749E4C68F9D7}" name="end_time" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{11F768A3-7132-674C-8E3C-457C09009AD5}" name="time_diff" dataDxfId="13">
       <calculatedColumnFormula>Table24511[[#This Row],[end_time]]-Table24511[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{6BF25E36-BEFE-334C-B53B-9359DA68008A}" name="notes"/>
@@ -881,9 +891,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{039AD6AB-0126-1947-A333-DE36DDA0B7E4}" name="Table245" displayName="Table245" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{8C37C915-F94A-5148-A3D1-EE8B899AF7F8}" name="start_time" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{B8735F0A-4AB0-C54D-85C0-1F0A63FA3498}" name="end_time" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{12E891A6-DF38-EE41-AC70-EAADDDA13272}" name="time_diff" dataDxfId="10">
       <calculatedColumnFormula>Table245[[#This Row],[end_time]]-Table245[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F8493A5C-0C25-FD45-A552-FE369F4F3DAD}" name="notes"/>
@@ -896,9 +906,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1825D363-0D01-614F-8BB6-B82D0839B62E}" name="Table245154" displayName="Table245154" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{85D813AA-3E14-AA49-8764-1AFB1744F6CB}" name="start_time" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{6FA6C7C4-391C-734C-A912-3190038D77AB}" name="end_time" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{9C4583F8-953A-D04B-AA91-7D77A5FF66F0}" name="time_diff" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{85D813AA-3E14-AA49-8764-1AFB1744F6CB}" name="start_time" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6FA6C7C4-391C-734C-A912-3190038D77AB}" name="end_time" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9C4583F8-953A-D04B-AA91-7D77A5FF66F0}" name="time_diff" dataDxfId="7">
       <calculatedColumnFormula>Table245154[[#This Row],[end_time]]-Table245154[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{23A25CAD-E05F-1648-AA7C-0B4BD9C1739D}" name="notes"/>
@@ -911,9 +921,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{CE45E49D-73E4-8A4C-B1C1-A5F171222BA6}" name="Table24515416" displayName="Table24515416" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{31B61C1F-509B-C549-8AEF-DF0658F2B96B}" name="start_time" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{091F6D25-E362-ED42-9029-E0BCEEAEA850}" name="end_time" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{318940A5-8075-5D4C-BD68-125D391D783D}" name="time_diff" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{31B61C1F-509B-C549-8AEF-DF0658F2B96B}" name="start_time" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{091F6D25-E362-ED42-9029-E0BCEEAEA850}" name="end_time" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{318940A5-8075-5D4C-BD68-125D391D783D}" name="time_diff" dataDxfId="4">
       <calculatedColumnFormula>Table24515416[[#This Row],[end_time]]-Table24515416[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{4ECB2A10-B67B-D84C-9D70-CB15A16921DE}" name="notes"/>
@@ -926,9 +936,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}" name="Table24515" displayName="Table24515" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{1A93302E-8621-7D48-88F2-5AC51E7EA3A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4542A81A-297E-DB48-B049-9309ACD42F2B}" name="start_time" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FC99294C-6B9C-9349-BAD2-0D219F840C1B}" name="end_time" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{DBC27D03-BB8D-904E-8022-8B6335C64879}" name="time_diff" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{4542A81A-297E-DB48-B049-9309ACD42F2B}" name="start_time" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FC99294C-6B9C-9349-BAD2-0D219F840C1B}" name="end_time" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{DBC27D03-BB8D-904E-8022-8B6335C64879}" name="time_diff" dataDxfId="1">
       <calculatedColumnFormula>Table24515[[#This Row],[end_time]]-Table24515[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{D5223D27-0D62-AC4C-857C-038DCA9594DB}" name="notes"/>
@@ -943,7 +953,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{01F56379-480D-E144-8844-79E29F338160}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{80A1EC3F-97BF-2A42-A823-A672AD58C802}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="35">
+    <tableColumn id="3" xr3:uid="{F529491E-B189-F14F-8D98-A6DD0470EB40}" name="time_diff" dataDxfId="36">
       <calculatedColumnFormula>Table2[[#This Row],[end_time]]-Table2[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DC0F7FFE-563B-3E40-AAB4-A68B98253F92}" name="notes"/>
@@ -958,7 +968,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7197966F-DB73-A94E-B2AE-FF5E410916CA}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{615965FE-9104-054A-86EF-13FD1960F3F6}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{B0854C19-C681-7640-AAB6-06872F731D13}" name="time_diff" dataDxfId="34">
+    <tableColumn id="3" xr3:uid="{B0854C19-C681-7640-AAB6-06872F731D13}" name="time_diff" dataDxfId="35">
       <calculatedColumnFormula>Table213[[#This Row],[end_time]]-Table213[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{0469E901-54FA-974D-A28F-40EC1AA491CD}" name="notes"/>
@@ -971,9 +981,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAC55445-B449-1B46-ADAD-5D1EE6A1BD3D}" name="Table246" displayName="Table246" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{54C1AFBA-849B-564E-9383-040E585C368C}" name="start_time" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{45F9645E-00F2-4A47-AB06-DBB721851807}" name="end_time" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{D8F0A3A2-BBC5-6D49-8527-799E99BCFA49}" name="time_diff" dataDxfId="32">
       <calculatedColumnFormula>Table246[[#This Row],[end_time]]-Table246[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{838825F0-239B-C440-9C0B-3A9D1E9C0D95}" name="notes"/>
@@ -988,7 +998,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{97B35572-DA30-684F-B3E5-729DB08045CE}" name="start_time"/>
     <tableColumn id="2" xr3:uid="{CB979489-F330-CB47-ACD8-45591E7E6177}" name="end_time"/>
-    <tableColumn id="3" xr3:uid="{C2A1FF6A-8B35-0348-85B8-BCECB7F2BCFE}" name="time_diff" dataDxfId="30">
+    <tableColumn id="3" xr3:uid="{C2A1FF6A-8B35-0348-85B8-BCECB7F2BCFE}" name="time_diff" dataDxfId="31">
       <calculatedColumnFormula>Table21314[[#This Row],[end_time]]-Table21314[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{C144438C-DE22-7644-A5DB-5310B9F06FD7}" name="notes"/>
@@ -1001,9 +1011,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7DEA103-B67A-0B49-99E5-BEE70970D4BB}" name="Table247" displayName="Table247" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{CB152735-EDBE-5144-8A33-370189AD9329}" name="start_time" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{78FDD20A-A666-E94B-A38C-0886D5E9FD55}" name="end_time" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{AE363FE2-700D-BC49-BD68-6E6DB6F05C17}" name="time_diff" dataDxfId="28">
       <calculatedColumnFormula>Table247[[#This Row],[end_time]]-Table247[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{CCA0740F-5707-C44E-AA57-B44DAE132805}" name="notes"/>
@@ -1016,9 +1026,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F5A4CEBC-9F74-3B4A-97EE-FBFC2B092D3F}" name="Table24812" displayName="Table24812" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{6B6BD5F2-A455-4741-BE8B-EB4069C30402}" name="start_time" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{1A57601A-180E-3841-905B-984320643C2E}" name="end_time" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00349B95-06C5-6347-9812-8CE148323ABF}" name="time_diff" dataDxfId="25">
       <calculatedColumnFormula>Table24812[[#This Row],[end_time]]-Table24812[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F0480389-BE2E-CA47-91C9-281947E722D0}" name="notes"/>
@@ -1031,9 +1041,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{772A68B7-3577-954E-96AB-3F9F135762FE}" name="Table248" displayName="Table248" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{6C1948AC-21BF-BA4D-A66C-95CD6D282814}" name="start_time" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{FCE64BF5-4264-4C43-929C-08AD08C28E78}" name="end_time" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{53FD3C4C-5892-8C4A-80B1-B3228D1980FF}" name="time_diff" dataDxfId="22">
       <calculatedColumnFormula>Table248[[#This Row],[end_time]]-Table248[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F22060DE-01C3-9C4C-A473-BCE8D37580D6}" name="notes"/>
@@ -1046,9 +1056,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D84B3EF0-7875-184B-870A-3642242A31F0}" name="Table2410" displayName="Table2410" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31" xr:uid="{7DCBAB66-89F8-6F47-8D64-FA0C26924201}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{3577E981-DDE4-CC47-8395-6FEE5951473E}" name="start_time" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{14BD1FB2-4172-BE43-8B3C-F4348552D39D}" name="end_time" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{EA005961-FE83-1F48-8259-AAAD2071A3B1}" name="time_diff" dataDxfId="19">
       <calculatedColumnFormula>Table2410[[#This Row],[end_time]]-Table2410[[#This Row],[start_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7A57ED91-2446-8F4F-95C2-3088CD96BD62}" name="notes"/>
@@ -2663,7 +2673,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,7 +3221,7 @@
         <v>47</v>
       </c>
       <c r="C35" s="5">
-        <v>0</v>
+        <v>0.73472222222222228</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3219,7 +3229,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <v>0</v>
+        <v>0.85069444444444442</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3228,7 +3238,7 @@
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>0</v>
+        <v>10020</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
@@ -3251,7 +3261,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3801,7 +3811,7 @@
         <v>47</v>
       </c>
       <c r="C35" s="5">
-        <v>0</v>
+        <v>0.57291666666666663</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,7 +3819,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <v>0</v>
+        <v>0.70416666666666672</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3818,7 +3828,7 @@
       </c>
       <c r="C37" s="6">
         <f>SUM(HOUR(C36-C35)*3600 + MINUTE(C36-C35)*60 + SECOND(C36-C35))</f>
-        <v>0</v>
+        <v>11340</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
@@ -4398,22 +4408,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F4A8F4-AAF9-534C-A76C-45D54A4AA321}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="53.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="3" max="6" width="11.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="53.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4430,16 +4440,19 @@
         <v>91</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -4455,17 +4468,17 @@
       <c r="E2" s="6">
         <v>6452</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -4481,15 +4494,15 @@
       <c r="E3" s="6">
         <v>5536</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -4502,17 +4515,17 @@
       <c r="E4" s="6">
         <v>5374</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -4528,28 +4541,28 @@
       <c r="E5" s="6">
         <v>8040</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -4565,15 +4578,15 @@
       <c r="E7" s="6">
         <v>2919</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -4589,17 +4602,17 @@
       <c r="E8" s="6">
         <v>2160</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
@@ -4615,15 +4628,15 @@
       <c r="E9" s="6">
         <v>4175</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
@@ -4639,143 +4652,161 @@
       <c r="E10" s="6">
         <v>1284</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="B11" s="6">
+        <v>10020</v>
+      </c>
       <c r="C11" s="6">
         <v>1478</v>
       </c>
+      <c r="D11" s="6">
+        <v>95</v>
+      </c>
       <c r="E11" s="6">
         <v>2938</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="B12" s="6">
+        <v>11340</v>
+      </c>
       <c r="C12" s="6">
         <v>2486</v>
       </c>
+      <c r="D12" s="6">
+        <v>165</v>
+      </c>
       <c r="E12" s="6">
         <v>3752</v>
       </c>
       <c r="F12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G37" s="4"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
-    <hyperlink ref="H5" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{3DBA40E2-94AD-4845-AA90-D92036F9A7B1}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{53E20B43-9ECF-BE46-AB3C-B2592713D701}"/>
+    <hyperlink ref="I8" r:id="rId1" xr:uid="{3970856A-E4AF-1A43-8B70-57FFA8C06E25}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{71A5A8C1-A76B-A547-AF17-C69B3E893425}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{DF7CF82C-9943-0245-B3E6-EDC7EA7731CC}"/>
+    <hyperlink ref="I4" r:id="rId4" xr:uid="{FBBBD265-3861-6B4B-9F87-EC807EFC88D7}"/>
+    <hyperlink ref="I5" r:id="rId5" xr:uid="{7A03C22B-A196-704B-A213-4637F9EBDC90}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{690F8EF1-089F-EC4D-A9A6-2859C8C8EB25}"/>
+    <hyperlink ref="I9" r:id="rId7" xr:uid="{3DBA40E2-94AD-4845-AA90-D92036F9A7B1}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{53E20B43-9ECF-BE46-AB3C-B2592713D701}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8693,6 +8724,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="3322fca5-43da-49d1-b081-466ee88b9b9d">
@@ -8701,15 +8741,6 @@
     <TaxCatchAll xmlns="08edd21d-9f77-405a-872a-1371c16ee465" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8732,6 +8763,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711BD0AE-A67E-4DE0-BFB7-7F2D919E2D80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -8746,12 +8785,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84C9AB0F-2376-4442-8FD0-7F9F6F9B731B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
We add in the IKEM data. This requires us to mix and match some metrics such as dwell time between the footage-derived number from Homolce with the GLG recorded metrics for everywhere else that we don't have footage available for. IKEM owes us some data still so the figures will change.
</commit_message>
<xml_diff>
--- a/data/raw/VCAS-I-rove_time.xlsx
+++ b/data/raw/VCAS-I-rove_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4209FB19-B9BD-B049-8C52-08734BE6231A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497194B8-90E2-864E-893B-23CE558211F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="34540" windowHeight="19920" activeTab="1" xr2:uid="{0490BC07-0248-8949-839E-74C08EF47166}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="124">
   <si>
     <t>Here we track total ablation time which I will refer to going forward as rove_time</t>
   </si>
@@ -244,9 +244,6 @@
   </si>
   <si>
     <t>This doesn't work correctly if done across days</t>
-  </si>
-  <si>
-    <t>num_applications</t>
   </si>
   <si>
     <t>procedure_time</t>
@@ -565,6 +562,12 @@
   </si>
   <si>
     <t>subjectId</t>
+  </si>
+  <si>
+    <t>numberlesions is number of locations where we ablated</t>
+  </si>
+  <si>
+    <t>numberapplications</t>
   </si>
 </sst>
 </file>
@@ -935,7 +938,7 @@
     <tableColumn id="1" xr3:uid="{718012BD-7025-314F-8E4E-E629C18A0C65}" name="subjectId" dataDxfId="61"/>
     <tableColumn id="7" xr3:uid="{C7BB62FA-ACAE-E548-9F55-EF382289F58E}" name="procedure_time" dataDxfId="60"/>
     <tableColumn id="2" xr3:uid="{461579DB-75ED-D945-B839-5CC1464620BE}" name="rove_time" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="num_applications" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{CDE9456B-9063-7C4C-B991-CBF83C4BD893}" name="numberapplications" dataDxfId="58"/>
     <tableColumn id="8" xr3:uid="{5E0CEC32-C01F-A446-827E-6309FE417F82}" name="dwell_time" dataDxfId="57">
       <calculatedColumnFormula>'1-001'!H35</calculatedColumnFormula>
     </tableColumn>
@@ -1579,10 +1582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535426F-7A8C-E949-810F-FB71A9FDBD02}">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="161" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1629,7 +1632,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -1639,57 +1642,62 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1748,7 +1756,7 @@
         <v>8.2870370370370372E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="14">
         <v>7.2511574074074076E-2</v>
@@ -1761,7 +1769,7 @@
         <v>1.4675925925925926E-2</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1776,7 +1784,7 @@
         <v>6.7824074074074314E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="16">
         <v>8.9803240740740739E-2</v>
@@ -1802,7 +1810,7 @@
         <v>7.0370370370369528E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -2204,14 +2212,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24511[time_diff]))*3600 + MINUTE(SUM(Table24511[time_diff])) * 60 + SECOND(SUM(Table24511[time_diff]))</f>
         <v>2043</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -2764,14 +2772,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245[time_diff]))*3600 + MINUTE(SUM(Table245[time_diff])) * 60 + SECOND(SUM(Table245[time_diff]))</f>
         <v>568</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -2895,7 +2903,7 @@
         <v>1.4918981481481408E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="14">
         <v>0.80343750000000003</v>
@@ -2921,7 +2929,7 @@
         <v>2.1875000000000089E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="16">
         <v>0.81846064814814812</v>
@@ -2934,7 +2942,7 @@
         <v>1.4780092592592609E-2</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -3370,14 +3378,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245154[time_diff]))*3600 + MINUTE(SUM(Table245154[time_diff])) * 60 + SECOND(SUM(Table245154[time_diff]))</f>
         <v>1478</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -3483,7 +3491,7 @@
         <v>1.8287037037036935E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="14">
         <v>0.64094907407407409</v>
@@ -3509,7 +3517,7 @@
         <v>6.5393518518518379E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" s="16">
         <v>0.6681597222222222</v>
@@ -3960,14 +3968,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515416[time_diff]))*3600 + MINUTE(SUM(Table24515416[time_diff])) * 60 + SECOND(SUM(Table24515416[time_diff]))</f>
         <v>2486</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -4079,7 +4087,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4526,14 +4534,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451517181920[time_diff]))*3600 + MINUTE(SUM(Table2451517181920[time_diff])) * 60 + SECOND(SUM(Table2451517181920[time_diff]))</f>
         <v>2808</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -4617,7 +4625,7 @@
         <v>3.4502314814814805E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -4626,7 +4634,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5077,14 +5085,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515171819[time_diff]))*3600 + MINUTE(SUM(Table24515171819[time_diff])) * 60 + SECOND(SUM(Table24515171819[time_diff]))</f>
         <v>3937</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -5168,7 +5176,7 @@
         <v>3.0567129629629652E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -5177,7 +5185,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5628,14 +5636,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245151718[time_diff]))*3600 + MINUTE(SUM(Table245151718[time_diff])) * 60 + SECOND(SUM(Table245151718[time_diff]))</f>
         <v>3340</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -5725,7 +5733,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -6176,14 +6184,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451517[time_diff]))*3600 + MINUTE(SUM(Table2451517[time_diff])) * 60 + SECOND(SUM(Table2451517[time_diff]))</f>
         <v>2171</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -6718,14 +6726,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2451521[time_diff]))*3600 + MINUTE(SUM(Table2451521[time_diff])) * 60 + SECOND(SUM(Table2451521[time_diff]))</f>
         <v>2594</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -7260,14 +7268,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table245152122[time_diff]))*3600 + MINUTE(SUM(Table245152122[time_diff])) * 60 + SECOND(SUM(Table245152122[time_diff]))</f>
         <v>935</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -7305,7 +7313,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7319,25 +7327,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
@@ -7363,10 +7371,10 @@
         <v>6452</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>16</v>
@@ -7392,10 +7400,10 @@
         <v>5536</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3" t="s">
@@ -7416,16 +7424,16 @@
         <v>5374</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -7445,13 +7453,13 @@
         <v>8040</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>13</v>
@@ -7486,10 +7494,10 @@
         <v>2919</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="8" t="s">
@@ -7513,21 +7521,21 @@
         <v>2160</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="6">
         <v>12840</v>
@@ -7542,19 +7550,19 @@
         <v>4175</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6">
         <v>9600</v>
@@ -7569,19 +7577,19 @@
         <v>1284</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="6">
         <v>10020</v>
@@ -7596,19 +7604,19 @@
         <v>2938</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="6">
         <v>11340</v>
@@ -7623,21 +7631,21 @@
         <v>3752</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="6">
         <v>2808</v>
@@ -7646,21 +7654,21 @@
         <v>139</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="6">
         <v>3937</v>
@@ -7669,19 +7677,19 @@
         <v>116</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="6">
         <v>3340</v>
@@ -7690,19 +7698,19 @@
         <v>143</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="6">
         <v>2171</v>
@@ -7711,19 +7719,19 @@
         <v>81</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" s="6">
         <v>2594</v>
@@ -7732,19 +7740,19 @@
         <v>105</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="6">
         <v>935</v>
@@ -7753,14 +7761,14 @@
         <v>40</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -8350,14 +8358,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24515[time_diff]))*3600 + MINUTE(SUM(Table24515[time_diff])) * 60 + SECOND(SUM(Table24515[time_diff]))</f>
         <v>0</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -8811,14 +8819,14 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2[time_diff]))*3600 + MINUTE(SUM(Table2[time_diff])) * 60 + SECOND(SUM(Table2[time_diff]))</f>
         <v>2801</v>
       </c>
       <c r="F33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H33" s="6">
         <f>HOUR(SUM(Table213[time_diff]))*3600 + MINUTE(SUM(Table213[time_diff])) * 60 + SECOND(SUM(Table213[time_diff]))</f>
@@ -8922,7 +8930,7 @@
         <v>1.4351851851851921E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="4">
         <v>9.087962962962963E-2</v>
@@ -8947,7 +8955,7 @@
         <v>4.1666666666666657E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H3" s="4">
         <f>Table21314[[#This Row],[end_time]]-Table21314[[#This Row],[start_time]]</f>
@@ -8966,7 +8974,7 @@
         <v>5.277777777777784E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -9342,14 +9350,14 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table246[time_diff]))*3600 + MINUTE(SUM(Table246[time_diff])) * 60 + SECOND(SUM(Table246[time_diff]))</f>
         <v>3965</v>
       </c>
       <c r="F33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H33" s="6">
         <f>HOUR(SUM(Table21314[time_diff]))*3600 + MINUTE(SUM(Table21314[time_diff])) * 60 + SECOND(SUM(Table21314[time_diff]))</f>
@@ -9488,7 +9496,7 @@
         <v>1.3425925925926174E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="16">
         <v>0.63871527777777781</v>
@@ -9514,7 +9522,7 @@
         <v>6.1111111111110672E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="14">
         <v>0.66612268518518514</v>
@@ -9540,7 +9548,7 @@
         <v>2.8819444444444448E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="16">
         <v>0.69787037037037036</v>
@@ -9926,14 +9934,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table247[time_diff]))*3600 + MINUTE(SUM(Table247[time_diff])) * 60 + SECOND(SUM(Table247[time_diff]))</f>
         <v>2075</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -10143,7 +10151,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -10284,7 +10292,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table24812[time_diff]))*3600 + MINUTE(SUM(Table24812[time_diff])) * 60 + SECOND(SUM(Table24812[time_diff]))</f>
@@ -10384,7 +10392,7 @@
         <v>2.418981481481508E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="14">
         <v>0.71141203703703704</v>
@@ -10410,7 +10418,7 @@
         <v>6.3888888888888884E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="16">
         <v>0.52440972222222226</v>
@@ -10434,7 +10442,7 @@
         <v>1.215277777777779E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -10839,14 +10847,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table248[time_diff]))*3600 + MINUTE(SUM(Table248[time_diff])) * 60 + SECOND(SUM(Table248[time_diff]))</f>
         <v>1993</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6" t="e">
@@ -11008,7 +11016,7 @@
         <v>1.4004629629629645E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -11412,14 +11420,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table2410[time_diff]))*3600 + MINUTE(SUM(Table2410[time_diff])) * 60 + SECOND(SUM(Table2410[time_diff]))</f>
         <v>1734</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">
@@ -11985,14 +11993,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6">
         <f>HOUR(SUM(Table249[time_diff]))*3600 + MINUTE(SUM(Table249[time_diff])) * 60 + SECOND(SUM(Table249[time_diff]))</f>
         <v>463</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="6">

</xml_diff>